<commit_message>
edited the script for closing excel application
</commit_message>
<xml_diff>
--- a/Tools/bug report tool.xlsx
+++ b/Tools/bug report tool.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rameshbabu-P\OneDrive\Patient Explorer Project\Tools\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rameshbabu-P\Documents\GitHub\PE\Tools\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="58">
   <si>
     <t>Bug Number</t>
   </si>
@@ -202,6 +202,9 @@
   </si>
   <si>
     <t>This bug is fixed please validate and close the bug. Thanks Rameshbabu</t>
+  </si>
+  <si>
+    <t>Close excel sheet after completion of test automation</t>
   </si>
 </sst>
 </file>
@@ -594,10 +597,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AK26"/>
+  <dimension ref="A1:AK27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="G28" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1286,6 +1289,29 @@
       </c>
       <c r="G26" t="s">
         <v>25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27" s="4">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>57</v>
+      </c>
+      <c r="C27" s="2">
+        <v>42559</v>
+      </c>
+      <c r="D27" t="s">
+        <v>12</v>
+      </c>
+      <c r="E27" t="s">
+        <v>52</v>
+      </c>
+      <c r="F27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G27" t="s">
+        <v>27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>